<commit_message>
extracting datasets details & other updates
</commit_message>
<xml_diff>
--- a/Data/DetList-TW.xlsx
+++ b/Data/DetList-TW.xlsx
@@ -1,226 +1,233 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uapt33090-my.sharepoint.com/personal/heliana_teixeira_ua_pt/Documents/Rdir/WFD-TRaC-data-upto2022/Data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_BC06933A1DD1E78472A4287467BB196192598F75" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{962D02E1-9F37-9442-A0FC-4E01160E7461}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="26520" yWindow="1840" windowWidth="20000" windowHeight="13460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
-  <si>
-    <t xml:space="preserve">observedPropertyDeterminandLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">observedPropertyDeterminandCode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resultUom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oxygen saturation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_3131-01-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAS_14797-55-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg{NO3}/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_3152-01-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[pH]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nitrite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAS_14797-65-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg{NO2}/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ammonium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAS_14798-03-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg{NH4}/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phosphate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAS_14265-44-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg{P}/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dissolved oxygen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_3132-01-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chlorophyll a</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_3164-01-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ug/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secchi depth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_3111-01-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salinity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_3141-01-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{PSU}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total nitrogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_31615-01-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg{N}/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total suspended solids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_31-02-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total phosphorus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAS_7723-14-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dissolved organic carbon (DOC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_3133-05-9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg{C}/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total organic carbon (TOC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_3133-06-0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chloride</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAS_16887-00-6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ammonia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAS_7664-41-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BOD5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_3133-01-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg{O2}/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Turbidity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_3112-01-4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{NTU}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total oxidised nitrogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_3161-02-2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-ionised ammonia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_31613-01-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mg{NH3}/L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total dissolved solids</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_31-03-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total inorganic nitrogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_3161-05-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total organic nitrogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EEA_3161-03-3</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="67">
+  <si>
+    <t>observedPropertyDeterminandLabel</t>
+  </si>
+  <si>
+    <t>observedPropertyDeterminandCode</t>
+  </si>
+  <si>
+    <t>resultUom</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>Oxygen saturation</t>
+  </si>
+  <si>
+    <t>EEA_3131-01-9</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Nitrate</t>
+  </si>
+  <si>
+    <t>CAS_14797-55-8</t>
+  </si>
+  <si>
+    <t>mg{NO3}/L</t>
+  </si>
+  <si>
+    <t>pH</t>
+  </si>
+  <si>
+    <t>EEA_3152-01-0</t>
+  </si>
+  <si>
+    <t>[pH]</t>
+  </si>
+  <si>
+    <t>Nitrite</t>
+  </si>
+  <si>
+    <t>CAS_14797-65-0</t>
+  </si>
+  <si>
+    <t>mg{NO2}/L</t>
+  </si>
+  <si>
+    <t>Ammonium</t>
+  </si>
+  <si>
+    <t>CAS_14798-03-9</t>
+  </si>
+  <si>
+    <t>mg{NH4}/L</t>
+  </si>
+  <si>
+    <t>Phosphate</t>
+  </si>
+  <si>
+    <t>CAS_14265-44-2</t>
+  </si>
+  <si>
+    <t>mg{P}/L</t>
+  </si>
+  <si>
+    <t>Dissolved oxygen</t>
+  </si>
+  <si>
+    <t>EEA_3132-01-2</t>
+  </si>
+  <si>
+    <t>mg/L</t>
+  </si>
+  <si>
+    <t>Chlorophyll a</t>
+  </si>
+  <si>
+    <t>EEA_3164-01-0</t>
+  </si>
+  <si>
+    <t>ug/L</t>
+  </si>
+  <si>
+    <t>Secchi depth</t>
+  </si>
+  <si>
+    <t>EEA_3111-01-1</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Salinity</t>
+  </si>
+  <si>
+    <t>EEA_3141-01-3</t>
+  </si>
+  <si>
+    <t>{PSU}</t>
+  </si>
+  <si>
+    <t>Total nitrogen</t>
+  </si>
+  <si>
+    <t>EEA_31615-01-7</t>
+  </si>
+  <si>
+    <t>mg{N}/L</t>
+  </si>
+  <si>
+    <t>Total suspended solids</t>
+  </si>
+  <si>
+    <t>EEA_31-02-7</t>
+  </si>
+  <si>
+    <t>Total phosphorus</t>
+  </si>
+  <si>
+    <t>CAS_7723-14-0</t>
+  </si>
+  <si>
+    <t>Dissolved organic carbon (DOC)</t>
+  </si>
+  <si>
+    <t>EEA_3133-05-9</t>
+  </si>
+  <si>
+    <t>mg{C}/L</t>
+  </si>
+  <si>
+    <t>Total organic carbon (TOC)</t>
+  </si>
+  <si>
+    <t>EEA_3133-06-0</t>
+  </si>
+  <si>
+    <t>Chloride</t>
+  </si>
+  <si>
+    <t>CAS_16887-00-6</t>
+  </si>
+  <si>
+    <t>Ammonia</t>
+  </si>
+  <si>
+    <t>CAS_7664-41-7</t>
+  </si>
+  <si>
+    <t>BOD5</t>
+  </si>
+  <si>
+    <t>EEA_3133-01-5</t>
+  </si>
+  <si>
+    <t>mg{O2}/L</t>
+  </si>
+  <si>
+    <t>Turbidity</t>
+  </si>
+  <si>
+    <t>EEA_3112-01-4</t>
+  </si>
+  <si>
+    <t>{NTU}</t>
+  </si>
+  <si>
+    <t>Total oxidised nitrogen</t>
+  </si>
+  <si>
+    <t>EEA_3161-02-2</t>
+  </si>
+  <si>
+    <t>Non-ionised ammonia</t>
+  </si>
+  <si>
+    <t>EEA_31613-01-1</t>
+  </si>
+  <si>
+    <t>mg{NH3}/L</t>
+  </si>
+  <si>
+    <t>Total dissolved solids</t>
+  </si>
+  <si>
+    <t>EEA_31-03-8</t>
+  </si>
+  <si>
+    <t>Total inorganic nitrogen</t>
+  </si>
+  <si>
+    <t>EEA_3161-05-5</t>
+  </si>
+  <si>
+    <t>Total organic nitrogen</t>
+  </si>
+  <si>
+    <t>EEA_3161-03-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -256,6 +263,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -537,14 +553,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -558,7 +580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -568,11 +590,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>1880</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -582,11 +604,11 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>1848</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -596,11 +618,11 @@
       <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>1842</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -610,11 +632,11 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>1798</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -624,11 +646,11 @@
       <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>1769</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -638,11 +660,11 @@
       <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>1734</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -652,11 +674,11 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="n">
+      <c r="D8">
         <v>1655</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -666,11 +688,11 @@
       <c r="C9" t="s">
         <v>27</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D9">
         <v>1484</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -680,11 +702,11 @@
       <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="D10" t="n">
+      <c r="D10">
         <v>1364</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -694,11 +716,11 @@
       <c r="C11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="n">
+      <c r="D11">
         <v>1250</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -708,11 +730,11 @@
       <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="D12" t="n">
+      <c r="D12">
         <v>943</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -722,11 +744,11 @@
       <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="D13" t="n">
+      <c r="D13">
         <v>916</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -736,11 +758,11 @@
       <c r="C14" t="s">
         <v>21</v>
       </c>
-      <c r="D14" t="n">
+      <c r="D14">
         <v>884</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -750,11 +772,11 @@
       <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="D15" t="n">
+      <c r="D15">
         <v>161</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -764,11 +786,11 @@
       <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="D16" t="n">
+      <c r="D16">
         <v>142</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>46</v>
       </c>
@@ -778,11 +800,11 @@
       <c r="C17" t="s">
         <v>24</v>
       </c>
-      <c r="D17" t="n">
+      <c r="D17">
         <v>140</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>48</v>
       </c>
@@ -792,11 +814,11 @@
       <c r="C18" t="s">
         <v>27</v>
       </c>
-      <c r="D18" t="n">
+      <c r="D18">
         <v>128</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>50</v>
       </c>
@@ -806,11 +828,11 @@
       <c r="C19" t="s">
         <v>52</v>
       </c>
-      <c r="D19" t="n">
+      <c r="D19">
         <v>125</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -820,11 +842,11 @@
       <c r="C20" t="s">
         <v>55</v>
       </c>
-      <c r="D20" t="n">
+      <c r="D20">
         <v>101</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -834,11 +856,11 @@
       <c r="C21" t="s">
         <v>36</v>
       </c>
-      <c r="D21" t="n">
+      <c r="D21">
         <v>83</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -848,11 +870,11 @@
       <c r="C22" t="s">
         <v>60</v>
       </c>
-      <c r="D22" t="n">
+      <c r="D22">
         <v>64</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -862,11 +884,11 @@
       <c r="C23" t="s">
         <v>24</v>
       </c>
-      <c r="D23" t="n">
+      <c r="D23">
         <v>34</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -876,11 +898,11 @@
       <c r="C24" t="s">
         <v>36</v>
       </c>
-      <c r="D24" t="n">
+      <c r="D24">
         <v>30</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -890,12 +912,12 @@
       <c r="C25" t="s">
         <v>36</v>
       </c>
-      <c r="D25" t="n">
+      <c r="D25">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>